<commit_message>
Final Adaptation for Proposalv05
</commit_message>
<xml_diff>
--- a/Data/Mapping_PPI_117grouping.xlsx
+++ b/Data/Mapping_PPI_117grouping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92558D5F-9E38-4B97-AA56-F5CE56F0AD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE53A30-1F31-4FCF-894A-B6D7C68F884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2295" windowWidth="18900" windowHeight="11025" xr2:uid="{EDFA86FE-7EC3-4BD5-B144-7D4F3B543281}"/>
+    <workbookView xWindow="-28920" yWindow="-435" windowWidth="29040" windowHeight="15840" xr2:uid="{EDFA86FE-7EC3-4BD5-B144-7D4F3B543281}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="147">
   <si>
     <t>CA Manufacture of food products, beverages and tobacco</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>CDE Manufacture of chemicals and oil refineries etc.</t>
-  </si>
-  <si>
-    <t>CE Manufacture of chemicals</t>
   </si>
   <si>
     <t>CF Pharmaceuticals</t>
@@ -872,43 +869,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8EE2BF-E3D1-42D8-8DDC-51452F7B04F5}">
   <dimension ref="B3:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122:XFD122"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -916,7 +914,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -924,7 +922,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -932,7 +930,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
@@ -940,7 +938,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
@@ -948,7 +946,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
@@ -956,7 +954,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -964,7 +962,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
@@ -972,7 +970,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -980,7 +978,7 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
@@ -988,7 +986,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -996,7 +994,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -1004,7 +1002,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
@@ -1012,7 +1010,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
@@ -1020,7 +1018,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
@@ -1028,7 +1026,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
@@ -1036,7 +1034,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -1044,7 +1042,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>10</v>
@@ -1052,7 +1050,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>10</v>
@@ -1060,7 +1058,7 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>11</v>
@@ -1068,778 +1066,778 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C72" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C75" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C76" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C77" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C79" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C90" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C92" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C96" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C99" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C101" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C102" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C104" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C105" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C106" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C107" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C108" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C110" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C111" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C112" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C113" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C114" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C115" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C116" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C117" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C118" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C119" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C120" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C121" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C122" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NACE and ISIC codes
</commit_message>
<xml_diff>
--- a/Data/Mapping_PPI_117grouping.xlsx
+++ b/Data/Mapping_PPI_117grouping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterThesis\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MasterThesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE53A30-1F31-4FCF-894A-B6D7C68F884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC6DA6C-DFF9-4C89-9FC3-78435D5CCB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-435" windowWidth="29040" windowHeight="15840" xr2:uid="{EDFA86FE-7EC3-4BD5-B144-7D4F3B543281}"/>
+    <workbookView xWindow="23880" yWindow="-3165" windowWidth="25440" windowHeight="15390" xr2:uid="{EDFA86FE-7EC3-4BD5-B144-7D4F3B543281}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="172">
   <si>
     <t>CA Manufacture of food products, beverages and tobacco</t>
   </si>
@@ -477,13 +477,88 @@
   </si>
   <si>
     <t>Class_output</t>
+  </si>
+  <si>
+    <t>ISIC_Code</t>
+  </si>
+  <si>
+    <t>ISIC_Name</t>
+  </si>
+  <si>
+    <t>Shapiro_Code</t>
+  </si>
+  <si>
+    <t>ZEW_Code</t>
+  </si>
+  <si>
+    <t>Food and beverages</t>
+  </si>
+  <si>
+    <t>Tobacco products</t>
+  </si>
+  <si>
+    <t>Textiles</t>
+  </si>
+  <si>
+    <t>Wearing apparel, fur</t>
+  </si>
+  <si>
+    <t>Leather, leather products and footwear</t>
+  </si>
+  <si>
+    <t>Wood products (excl. furniture)</t>
+  </si>
+  <si>
+    <t>Paper and paper products</t>
+  </si>
+  <si>
+    <t>Printing and publishing</t>
+  </si>
+  <si>
+    <t>Coke,refined petroleum products,nuclear fuel</t>
+  </si>
+  <si>
+    <t>Chemicals and chemical products</t>
+  </si>
+  <si>
+    <t>Rubber and plastics products</t>
+  </si>
+  <si>
+    <t>Non-metallic mineral products</t>
+  </si>
+  <si>
+    <t>Basic metals</t>
+  </si>
+  <si>
+    <t>Fabricated metal products</t>
+  </si>
+  <si>
+    <t>Machinery and equipment n.e.c.</t>
+  </si>
+  <si>
+    <t>Furniture; manufacturing n.e.c.</t>
+  </si>
+  <si>
+    <t>Motor vehicles, trailers, semi-trailers</t>
+  </si>
+  <si>
+    <t>Other transport equipment</t>
+  </si>
+  <si>
+    <t>Medical, precision and optical instruments</t>
+  </si>
+  <si>
+    <t>Electrical machinery and apparatus</t>
+  </si>
+  <si>
+    <t>Office, accounting and computing machinery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,6 +584,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -538,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -552,6 +635,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -867,28 +968,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8EE2BF-E3D1-42D8-8DDC-51452F7B04F5}">
-  <dimension ref="B3:C122"/>
+  <dimension ref="B3:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>144</v>
       </c>
@@ -896,7 +1010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
@@ -904,7 +1018,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -912,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
@@ -920,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
@@ -928,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -936,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -944,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -952,287 +1066,707 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="8">
+        <v>17</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="10">
+        <v>2</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="8">
+        <v>18</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="10">
+        <v>2</v>
+      </c>
+      <c r="G20" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="8">
+        <v>19</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="10">
+        <v>2</v>
+      </c>
+      <c r="G21" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="8">
+        <v>20</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="10">
+        <v>3</v>
+      </c>
+      <c r="G22" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="8">
+        <v>21</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="10">
+        <v>4</v>
+      </c>
+      <c r="G23" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="8">
+        <v>22</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="10">
+        <v>4</v>
+      </c>
+      <c r="G24" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="8">
+        <v>23</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="10">
+        <v>5</v>
+      </c>
+      <c r="G25" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="8">
+        <v>24</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="8">
+        <v>24</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="8">
+        <v>24</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="8">
+        <v>25</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="8">
+        <v>26</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="8">
+        <v>26</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="8">
+        <v>27</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="11">
+        <v>28</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" s="12">
+        <v>10</v>
+      </c>
+      <c r="G33" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="7">
+        <v>30</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F34">
+        <v>12.13</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="7">
+        <v>30</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35">
+        <v>12.13</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="8">
+        <v>31</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="10">
+        <v>12</v>
+      </c>
+      <c r="G36" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="8">
+        <v>31</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="10">
+        <v>12</v>
+      </c>
+      <c r="G37" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="8">
+        <v>31</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="10">
+        <v>12</v>
+      </c>
+      <c r="G38" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="7">
+        <v>29</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F39">
+        <v>11</v>
+      </c>
+      <c r="G39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="7">
+        <v>29</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F40">
+        <v>11</v>
+      </c>
+      <c r="G40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="8">
+        <v>34</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" s="10">
+        <v>15</v>
+      </c>
+      <c r="G41" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="7">
+        <v>35</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F42">
+        <v>16</v>
+      </c>
+      <c r="G42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="7">
+        <v>36</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F43">
+        <v>17</v>
+      </c>
+      <c r="G43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="8">
+        <v>33</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F44" s="10">
+        <v>14</v>
+      </c>
+      <c r="G44" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="7">
+        <v>36</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F45">
+        <v>17</v>
+      </c>
+      <c r="G45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="7">
+        <v>29</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F46">
+        <v>11</v>
+      </c>
+      <c r="G46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>68</v>
       </c>
@@ -1240,7 +1774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Add ZEW classification data
</commit_message>
<xml_diff>
--- a/Data/Mapping_PPI_117grouping.xlsx
+++ b/Data/Mapping_PPI_117grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MasterThesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC6DA6C-DFF9-4C89-9FC3-78435D5CCB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39B8362-4FC0-494A-ADEB-A272773CD4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-3165" windowWidth="25440" windowHeight="15390" xr2:uid="{EDFA86FE-7EC3-4BD5-B144-7D4F3B543281}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="184">
   <si>
     <t>CA Manufacture of food products, beverages and tobacco</t>
   </si>
@@ -552,6 +552,42 @@
   </si>
   <si>
     <t>Office, accounting and computing machinery</t>
+  </si>
+  <si>
+    <t>ZEW_Name</t>
+  </si>
+  <si>
+    <t>food, tobacco, beverages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">textiles, wearing apparel, leather </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wood products </t>
+  </si>
+  <si>
+    <t>pulp, paper, publishing</t>
+  </si>
+  <si>
+    <t>coke, petroleum</t>
+  </si>
+  <si>
+    <t>chemicals, pharmaceuticals</t>
+  </si>
+  <si>
+    <t>rubber, plastics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-metallic minerals </t>
+  </si>
+  <si>
+    <t>metals</t>
+  </si>
+  <si>
+    <t>metal products, electronics, machinery</t>
+  </si>
+  <si>
+    <t>vehicles, other transport, n.e.c.</t>
   </si>
 </sst>
 </file>
@@ -621,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -648,11 +684,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -968,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8EE2BF-E3D1-42D8-8DDC-51452F7B04F5}">
-  <dimension ref="B3:G122"/>
+  <dimension ref="B3:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,10 +1010,10 @@
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>146</v>
       </c>
@@ -1001,8 +1032,11 @@
       <c r="G3" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>144</v>
       </c>
@@ -1010,7 +1044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1018,7 +1052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1026,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1034,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1042,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1050,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1058,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1066,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1085,8 +1119,11 @@
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1105,8 +1142,11 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1125,8 +1165,11 @@
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1145,8 +1188,11 @@
       <c r="G15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1165,8 +1211,11 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1185,8 +1234,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1205,8 +1257,11 @@
       <c r="G18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
@@ -1219,14 +1274,17 @@
       <c r="E19" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19">
         <v>2</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
@@ -1239,14 +1297,17 @@
       <c r="E20" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20">
         <v>2</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1259,14 +1320,17 @@
       <c r="E21" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21">
         <v>2</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1279,14 +1343,17 @@
       <c r="E22" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22">
         <v>3</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1299,14 +1366,17 @@
       <c r="E23" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23">
         <v>4</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>45</v>
       </c>
@@ -1319,14 +1389,17 @@
       <c r="E24" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24">
         <v>4</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1339,14 +1412,17 @@
       <c r="E25" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25">
         <v>5</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1365,8 +1441,11 @@
       <c r="G26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
@@ -1385,8 +1464,11 @@
       <c r="G27">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1405,8 +1487,11 @@
       <c r="G28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1425,8 +1510,11 @@
       <c r="G29">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1445,8 +1533,11 @@
       <c r="G30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
@@ -1465,8 +1556,11 @@
       <c r="G31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
@@ -1485,28 +1579,34 @@
       <c r="G32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="7">
         <v>28</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33">
         <v>10</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
@@ -1525,8 +1625,11 @@
       <c r="G34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
@@ -1545,8 +1648,11 @@
       <c r="G35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>57</v>
       </c>
@@ -1559,14 +1665,17 @@
       <c r="E36" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36">
         <v>12</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>58</v>
       </c>
@@ -1579,14 +1688,17 @@
       <c r="E37" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37">
         <v>12</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>59</v>
       </c>
@@ -1599,14 +1711,17 @@
       <c r="E38" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38">
         <v>12</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>60</v>
       </c>
@@ -1625,8 +1740,11 @@
       <c r="G39">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>61</v>
       </c>
@@ -1645,8 +1763,11 @@
       <c r="G40">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
@@ -1659,14 +1780,17 @@
       <c r="E41" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F41">
         <v>15</v>
       </c>
-      <c r="G41" s="10">
+      <c r="G41">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
@@ -1685,8 +1809,11 @@
       <c r="G42">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>64</v>
       </c>
@@ -1705,8 +1832,11 @@
       <c r="G43">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1719,14 +1849,17 @@
       <c r="E44" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F44">
         <v>14</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G44">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>66</v>
       </c>
@@ -1745,8 +1878,11 @@
       <c r="G45">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>67</v>
       </c>
@@ -1765,8 +1901,11 @@
       <c r="G46">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>68</v>
       </c>
@@ -1774,7 +1913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>